<commit_message>
Added TICC-219 identifiers; Advanced Ordering
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.3.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E332F360-767C-45BF-9F07-B0BB059D0EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6100C900-C1FF-4C02-B528-23042F262BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="1110" windowWidth="26340" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -27,20 +27,11 @@
     <definedName name="_ftnref4" localSheetId="0">'Document Type'!$A$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="526">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1615,6 +1606,39 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:fdc:peppol:jp:billing:3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderChange-2::OrderChange##urn:fdc:peppol.eu:poacc:trns:order_change:3::2.3</t>
+  </si>
+  <si>
+    <t>TICC-219</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:advanced_ordering:3</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderCancellation-2::OrderCancellation##urn:fdc:peppol.eu:poacc:trns:order_cancellation:3::2.3</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:OrderResponse-2::OrderResponse##urn:fdc:peppol.eu:poacc:trns:order_response_advanced:3::2.3</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:fdc:peppol.eu:poacc:trns:order:3::2.3</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>Peppol Order Change</t>
+  </si>
+  <si>
+    <t>Peppol Order Cancellation</t>
+  </si>
+  <si>
+    <t>Peppol Order Response Advanced</t>
+  </si>
+  <si>
+    <t>Peppol Order Advanced</t>
   </si>
 </sst>
 </file>
@@ -1717,68 +1741,61 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2197,11 +2214,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L187"/>
+  <dimension ref="A1:L191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A191" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2209,10 +2226,10 @@
     <col min="1" max="1" width="47.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="103.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="6" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="5"/>
@@ -2231,16 +2248,16 @@
       <c r="C1" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>431</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="14" t="s">
         <v>430</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -2269,7 +2286,7 @@
       <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -2302,7 +2319,7 @@
       <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -2335,7 +2352,7 @@
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -2368,7 +2385,7 @@
       <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -2401,7 +2418,7 @@
       <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -2434,7 +2451,7 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -2467,7 +2484,7 @@
       <c r="C8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -2500,7 +2517,7 @@
       <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -2533,7 +2550,7 @@
       <c r="C10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -2569,7 +2586,7 @@
       <c r="C11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="19">
         <v>3</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -2602,7 +2619,7 @@
       <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -2635,7 +2652,7 @@
       <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -2668,7 +2685,7 @@
       <c r="C14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -2701,7 +2718,7 @@
       <c r="C15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -2734,7 +2751,7 @@
       <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="19" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -2767,7 +2784,7 @@
       <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -2800,7 +2817,7 @@
       <c r="C18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -2833,7 +2850,7 @@
       <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2866,7 +2883,7 @@
       <c r="C20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -2899,7 +2916,7 @@
       <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -2932,7 +2949,7 @@
       <c r="C22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -2965,7 +2982,7 @@
       <c r="C23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -2998,7 +3015,7 @@
       <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="18" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -3031,7 +3048,7 @@
       <c r="C25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="19" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -3061,7 +3078,7 @@
       <c r="C26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="19" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -3088,7 +3105,7 @@
       <c r="C27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -3121,7 +3138,7 @@
       <c r="C28" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -3157,7 +3174,7 @@
       <c r="C29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="19">
         <v>3</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -3190,7 +3207,7 @@
       <c r="C30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -3223,7 +3240,7 @@
       <c r="C31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="19" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -3256,7 +3273,7 @@
       <c r="C32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="18">
         <v>2</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -3286,7 +3303,7 @@
       <c r="C33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="18">
         <v>2</v>
       </c>
       <c r="E33" s="5" t="s">
@@ -3316,7 +3333,7 @@
       <c r="C34" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="19">
         <v>3</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -3343,7 +3360,7 @@
       <c r="C35" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="19">
         <v>3</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -3376,7 +3393,7 @@
       <c r="C36" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E36" s="5" t="s">
@@ -3406,7 +3423,7 @@
       <c r="C37" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="18">
         <v>3</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -3436,7 +3453,7 @@
       <c r="C38" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="18">
         <v>3</v>
       </c>
       <c r="E38" s="5" t="s">
@@ -3466,7 +3483,7 @@
       <c r="C39" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="18">
         <v>3</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -3496,7 +3513,7 @@
       <c r="C40" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="18">
         <v>3</v>
       </c>
       <c r="E40" s="5" t="s">
@@ -3526,7 +3543,7 @@
       <c r="C41" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="21">
+      <c r="D41" s="18">
         <v>3</v>
       </c>
       <c r="E41" s="5" t="s">
@@ -3556,7 +3573,7 @@
       <c r="C42" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="18">
         <v>3</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -3586,7 +3603,7 @@
       <c r="C43" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="21">
+      <c r="D43" s="18">
         <v>3</v>
       </c>
       <c r="E43" s="5" t="s">
@@ -3616,7 +3633,7 @@
       <c r="C44" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="21">
+      <c r="D44" s="18">
         <v>3</v>
       </c>
       <c r="E44" s="5" t="s">
@@ -3649,7 +3666,7 @@
       <c r="C45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="21">
+      <c r="D45" s="18">
         <v>3</v>
       </c>
       <c r="E45" s="5" t="s">
@@ -3682,7 +3699,7 @@
       <c r="C46" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="18">
         <v>3</v>
       </c>
       <c r="E46" s="5" t="s">
@@ -3715,7 +3732,7 @@
       <c r="C47" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="18">
         <v>3</v>
       </c>
       <c r="E47" s="5" t="s">
@@ -3745,7 +3762,7 @@
       <c r="C48" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="18">
         <v>3</v>
       </c>
       <c r="E48" s="5" t="s">
@@ -3775,7 +3792,7 @@
       <c r="C49" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="18">
         <v>3</v>
       </c>
       <c r="E49" s="5" t="s">
@@ -3805,7 +3822,7 @@
       <c r="C50" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="18">
         <v>3</v>
       </c>
       <c r="E50" s="5" t="s">
@@ -3835,7 +3852,7 @@
       <c r="C51" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="21">
+      <c r="D51" s="18">
         <v>4</v>
       </c>
       <c r="E51" s="5" t="s">
@@ -3868,7 +3885,7 @@
       <c r="C52" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D52" s="21">
+      <c r="D52" s="18">
         <v>4</v>
       </c>
       <c r="E52" s="5" t="s">
@@ -3898,7 +3915,7 @@
       <c r="C53" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D53" s="21">
+      <c r="D53" s="18">
         <v>4</v>
       </c>
       <c r="E53" s="5" t="s">
@@ -3928,7 +3945,7 @@
       <c r="C54" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D54" s="21">
+      <c r="D54" s="18">
         <v>4</v>
       </c>
       <c r="E54" s="5" t="s">
@@ -3958,7 +3975,7 @@
       <c r="C55" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="21">
+      <c r="D55" s="18">
         <v>4</v>
       </c>
       <c r="E55" s="5" t="s">
@@ -3988,7 +4005,7 @@
       <c r="C56" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D56" s="21">
+      <c r="D56" s="18">
         <v>4</v>
       </c>
       <c r="E56" s="5" t="s">
@@ -4018,7 +4035,7 @@
       <c r="C57" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D57" s="21">
+      <c r="D57" s="18">
         <v>4</v>
       </c>
       <c r="E57" s="5" t="s">
@@ -4048,7 +4065,7 @@
       <c r="C58" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D58" s="21">
+      <c r="D58" s="18">
         <v>4</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -4078,7 +4095,7 @@
       <c r="C59" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D59" s="21">
+      <c r="D59" s="18">
         <v>4</v>
       </c>
       <c r="E59" s="5" t="s">
@@ -4108,7 +4125,7 @@
       <c r="C60" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D60" s="21">
+      <c r="D60" s="18">
         <v>4</v>
       </c>
       <c r="E60" s="5" t="s">
@@ -4138,7 +4155,7 @@
       <c r="C61" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="21">
+      <c r="D61" s="18">
         <v>4</v>
       </c>
       <c r="E61" s="5" t="s">
@@ -4165,7 +4182,7 @@
       <c r="C62" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D62" s="21">
+      <c r="D62" s="18">
         <v>4</v>
       </c>
       <c r="E62" s="5" t="s">
@@ -4192,7 +4209,7 @@
       <c r="C63" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="21">
+      <c r="D63" s="18">
         <v>4</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -4222,7 +4239,7 @@
       <c r="C64" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D64" s="21">
+      <c r="D64" s="18">
         <v>4</v>
       </c>
       <c r="E64" s="5" t="s">
@@ -4258,7 +4275,7 @@
       <c r="C65" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D65" s="21">
+      <c r="D65" s="18">
         <v>6</v>
       </c>
       <c r="E65" s="5" t="s">
@@ -4291,7 +4308,7 @@
       <c r="C66" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D66" s="21">
+      <c r="D66" s="18">
         <v>5</v>
       </c>
       <c r="E66" s="5" t="s">
@@ -4321,7 +4338,7 @@
       <c r="C67" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D67" s="21">
+      <c r="D67" s="18">
         <v>5</v>
       </c>
       <c r="E67" s="5" t="s">
@@ -4351,7 +4368,7 @@
       <c r="C68" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D68" s="21">
+      <c r="D68" s="18">
         <v>5</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -4381,7 +4398,7 @@
       <c r="C69" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D69" s="21">
+      <c r="D69" s="18">
         <v>6</v>
       </c>
       <c r="E69" s="5" t="s">
@@ -4411,7 +4428,7 @@
       <c r="C70" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D70" s="21">
+      <c r="D70" s="18">
         <v>6</v>
       </c>
       <c r="E70" s="5" t="s">
@@ -4441,7 +4458,7 @@
       <c r="C71" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D71" s="21">
+      <c r="D71" s="18">
         <v>6</v>
       </c>
       <c r="E71" s="5" t="s">
@@ -4462,7 +4479,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" ht="45">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="1" t="s">
         <v>494</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -4471,7 +4488,7 @@
       <c r="C72" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D72" s="21">
+      <c r="D72" s="18">
         <v>6</v>
       </c>
       <c r="E72" s="5" t="s">
@@ -4495,7 +4512,7 @@
       </c>
     </row>
     <row r="73" spans="1:12" ht="45">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="1" t="s">
         <v>495</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -4504,7 +4521,7 @@
       <c r="C73" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D73" s="21">
+      <c r="D73" s="18">
         <v>6</v>
       </c>
       <c r="E73" s="5" t="s">
@@ -4537,7 +4554,7 @@
       <c r="C74" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D74" s="21">
+      <c r="D74" s="18">
         <v>6</v>
       </c>
       <c r="E74" s="5" t="s">
@@ -4567,7 +4584,7 @@
       <c r="C75" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D75" s="21">
+      <c r="D75" s="18">
         <v>6</v>
       </c>
       <c r="E75" s="5" t="s">
@@ -4597,7 +4614,7 @@
       <c r="C76" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D76" s="21">
+      <c r="D76" s="18">
         <v>6</v>
       </c>
       <c r="E76" s="5" t="s">
@@ -4627,7 +4644,7 @@
       <c r="C77" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D77" s="21">
+      <c r="D77" s="18">
         <v>6</v>
       </c>
       <c r="E77" s="5" t="s">
@@ -4657,16 +4674,16 @@
       <c r="C78" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D78" s="21">
+      <c r="D78" s="18">
         <v>7</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="F78" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G78" s="19"/>
+      <c r="G78" s="16"/>
       <c r="H78" s="5" t="s">
         <v>220</v>
       </c>
@@ -4691,16 +4708,16 @@
       <c r="C79" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D79" s="21">
+      <c r="D79" s="18">
         <v>7</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="F79" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G79" s="19"/>
+      <c r="G79" s="16"/>
       <c r="H79" s="5" t="s">
         <v>220</v>
       </c>
@@ -4725,16 +4742,16 @@
       <c r="C80" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D80" s="21">
+      <c r="D80" s="18">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F80" s="9" t="s">
+      <c r="F80" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G80" s="19"/>
+      <c r="G80" s="16"/>
       <c r="H80" s="5" t="s">
         <v>220</v>
       </c>
@@ -4759,7 +4776,7 @@
       <c r="C81" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D81" s="21">
+      <c r="D81" s="18">
         <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
@@ -4789,7 +4806,7 @@
       <c r="C82" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D82" s="21">
+      <c r="D82" s="18">
         <v>7</v>
       </c>
       <c r="E82" s="5" t="s">
@@ -4819,16 +4836,16 @@
       <c r="C83" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D83" s="21">
+      <c r="D83" s="18">
         <v>7</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F83" s="10" t="s">
+      <c r="F83" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="G83" s="19"/>
+      <c r="G83" s="16"/>
       <c r="H83" s="5" t="s">
         <v>214</v>
       </c>
@@ -4853,7 +4870,7 @@
       <c r="C84" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D84" s="22" t="s">
+      <c r="D84" s="19" t="s">
         <v>247</v>
       </c>
       <c r="E84" s="5" t="s">
@@ -4883,16 +4900,16 @@
       <c r="C85" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D85" s="21">
+      <c r="D85" s="18">
         <v>7</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F85" s="9" t="s">
+      <c r="F85" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G85" s="19"/>
+      <c r="G85" s="16"/>
       <c r="H85" s="5" t="s">
         <v>210</v>
       </c>
@@ -4917,16 +4934,16 @@
       <c r="C86" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D86" s="21">
+      <c r="D86" s="18">
         <v>7</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="F86" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G86" s="19"/>
+      <c r="G86" s="16"/>
       <c r="H86" s="5" t="s">
         <v>210</v>
       </c>
@@ -4951,16 +4968,16 @@
       <c r="C87" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D87" s="21">
+      <c r="D87" s="18">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F87" s="9" t="s">
+      <c r="F87" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G87" s="19"/>
+      <c r="G87" s="16"/>
       <c r="H87" s="5" t="s">
         <v>210</v>
       </c>
@@ -4985,7 +5002,7 @@
       <c r="C88" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D88" s="21">
+      <c r="D88" s="18">
         <v>7</v>
       </c>
       <c r="E88" s="5" t="s">
@@ -5015,16 +5032,16 @@
       <c r="C89" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D89" s="21">
+      <c r="D89" s="18">
         <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F89" s="10" t="s">
+      <c r="F89" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="G89" s="19"/>
+      <c r="G89" s="16"/>
       <c r="H89" s="5" t="s">
         <v>212</v>
       </c>
@@ -5049,16 +5066,16 @@
       <c r="C90" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D90" s="21">
+      <c r="D90" s="18">
         <v>7</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F90" s="10" t="s">
+      <c r="F90" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="G90" s="19"/>
+      <c r="G90" s="16"/>
       <c r="H90" s="5" t="s">
         <v>212</v>
       </c>
@@ -5083,16 +5100,16 @@
       <c r="C91" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D91" s="21">
+      <c r="D91" s="18">
         <v>7</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="F91" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="G91" s="19"/>
+      <c r="G91" s="16"/>
       <c r="H91" s="5" t="s">
         <v>212</v>
       </c>
@@ -5117,16 +5134,16 @@
       <c r="C92" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D92" s="21">
+      <c r="D92" s="18">
         <v>7</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F92" s="10" t="s">
+      <c r="F92" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="G92" s="19"/>
+      <c r="G92" s="16"/>
       <c r="H92" s="5" t="s">
         <v>212</v>
       </c>
@@ -5151,7 +5168,7 @@
       <c r="C93" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D93" s="21">
+      <c r="D93" s="18">
         <v>7</v>
       </c>
       <c r="E93" s="5" t="s">
@@ -5181,7 +5198,7 @@
       <c r="C94" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D94" s="21">
+      <c r="D94" s="18">
         <v>7</v>
       </c>
       <c r="E94" s="5" t="s">
@@ -5211,7 +5228,7 @@
       <c r="C95" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="D95" s="21">
+      <c r="D95" s="18">
         <v>7</v>
       </c>
       <c r="E95" s="5" t="s">
@@ -5241,7 +5258,7 @@
       <c r="C96" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D96" s="22" t="s">
+      <c r="D96" s="19" t="s">
         <v>207</v>
       </c>
       <c r="E96" s="5" t="s">
@@ -5271,7 +5288,7 @@
       <c r="C97" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D97" s="22" t="s">
+      <c r="D97" s="19" t="s">
         <v>207</v>
       </c>
       <c r="E97" s="5" t="s">
@@ -5301,16 +5318,16 @@
       <c r="C98" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="D98" s="22" t="s">
+      <c r="D98" s="19" t="s">
         <v>207</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="F98" s="10" t="s">
+      <c r="F98" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="G98" s="19"/>
+      <c r="G98" s="16"/>
       <c r="H98" s="5" t="s">
         <v>370</v>
       </c>
@@ -5335,7 +5352,7 @@
       <c r="C99" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="D99" s="22" t="s">
+      <c r="D99" s="19" t="s">
         <v>247</v>
       </c>
       <c r="E99" s="5" t="s">
@@ -5365,7 +5382,7 @@
       <c r="C100" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D100" s="22" t="s">
+      <c r="D100" s="19" t="s">
         <v>207</v>
       </c>
       <c r="E100" s="5" t="s">
@@ -5395,7 +5412,7 @@
       <c r="C101" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D101" s="22" t="s">
+      <c r="D101" s="19" t="s">
         <v>207</v>
       </c>
       <c r="E101" s="5" t="s">
@@ -5416,16 +5433,16 @@
       </c>
     </row>
     <row r="102" spans="1:12" ht="45">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="B102" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C102" s="11" t="s">
+      <c r="B102" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="D102" s="22" t="s">
+      <c r="D102" s="19" t="s">
         <v>230</v>
       </c>
       <c r="E102" s="5" t="s">
@@ -5441,7 +5458,7 @@
       <c r="K102" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L102" s="13" t="s">
+      <c r="L102" s="12" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5449,13 +5466,13 @@
       <c r="A103" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B103" s="12" t="s">
+      <c r="B103" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="D103" s="22" t="s">
+      <c r="D103" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E103" s="5" t="s">
@@ -5482,7 +5499,7 @@
       <c r="C104" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D104" s="22" t="s">
+      <c r="D104" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E104" s="5" t="s">
@@ -5512,7 +5529,7 @@
       <c r="C105" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D105" s="22" t="s">
+      <c r="D105" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E105" s="5" t="s">
@@ -5542,7 +5559,7 @@
       <c r="C106" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D106" s="22" t="s">
+      <c r="D106" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E106" s="5" t="s">
@@ -5572,7 +5589,7 @@
       <c r="C107" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="D107" s="22" t="s">
+      <c r="D107" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E107" s="5" t="s">
@@ -5596,13 +5613,13 @@
       <c r="A108" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="B108" t="s">
         <v>56</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D108" s="22" t="s">
+      <c r="D108" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E108" s="5" t="s">
@@ -5615,7 +5632,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K108" s="14" t="s">
+      <c r="K108" t="s">
         <v>371</v>
       </c>
       <c r="L108" s="5" t="s">
@@ -5626,13 +5643,13 @@
       <c r="A109" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="B109" t="s">
         <v>56</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D109" s="22" t="s">
+      <c r="D109" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E109" s="5" t="s">
@@ -5645,7 +5662,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K109" s="14" t="s">
+      <c r="K109" t="s">
         <v>371</v>
       </c>
       <c r="L109" s="5" t="s">
@@ -5656,13 +5673,13 @@
       <c r="A110" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B110" t="s">
         <v>56</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D110" s="22" t="s">
+      <c r="D110" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E110" s="5" t="s">
@@ -5675,7 +5692,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K110" s="14" t="s">
+      <c r="K110" t="s">
         <v>371</v>
       </c>
       <c r="L110" s="5" t="s">
@@ -5686,13 +5703,13 @@
       <c r="A111" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="B111" t="s">
         <v>56</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D111" s="22" t="s">
+      <c r="D111" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E111" s="5" t="s">
@@ -5705,7 +5722,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K111" s="14" t="s">
+      <c r="K111" t="s">
         <v>371</v>
       </c>
       <c r="L111" s="5" t="s">
@@ -5716,13 +5733,13 @@
       <c r="A112" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="B112" t="s">
         <v>56</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D112" s="22" t="s">
+      <c r="D112" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E112" s="5" t="s">
@@ -5735,7 +5752,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K112" s="14" t="s">
+      <c r="K112" t="s">
         <v>371</v>
       </c>
       <c r="L112" s="5" t="s">
@@ -5746,13 +5763,13 @@
       <c r="A113" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B113" t="s">
         <v>56</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D113" s="22" t="s">
+      <c r="D113" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E113" s="5" t="s">
@@ -5765,7 +5782,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K113" s="14" t="s">
+      <c r="K113" t="s">
         <v>371</v>
       </c>
       <c r="L113" s="5" t="s">
@@ -5776,13 +5793,13 @@
       <c r="A114" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="B114" t="s">
         <v>56</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D114" s="22" t="s">
+      <c r="D114" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E114" s="5" t="s">
@@ -5795,7 +5812,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K114" s="14" t="s">
+      <c r="K114" t="s">
         <v>371</v>
       </c>
       <c r="L114" s="5" t="s">
@@ -5806,13 +5823,13 @@
       <c r="A115" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B115" s="14" t="s">
+      <c r="B115" t="s">
         <v>56</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D115" s="22" t="s">
+      <c r="D115" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E115" s="5" t="s">
@@ -5825,7 +5842,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K115" s="14" t="s">
+      <c r="K115" t="s">
         <v>371</v>
       </c>
       <c r="L115" s="5" t="s">
@@ -5836,13 +5853,13 @@
       <c r="A116" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="B116" t="s">
         <v>56</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D116" s="22" t="s">
+      <c r="D116" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E116" s="5" t="s">
@@ -5855,7 +5872,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K116" s="14" t="s">
+      <c r="K116" t="s">
         <v>371</v>
       </c>
       <c r="L116" s="5" t="s">
@@ -5866,13 +5883,13 @@
       <c r="A117" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="B117" t="s">
         <v>56</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D117" s="22" t="s">
+      <c r="D117" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E117" s="5" t="s">
@@ -5885,7 +5902,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K117" s="14" t="s">
+      <c r="K117" t="s">
         <v>371</v>
       </c>
       <c r="L117" s="5" t="s">
@@ -5896,13 +5913,13 @@
       <c r="A118" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B118" s="14" t="s">
+      <c r="B118" t="s">
         <v>56</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D118" s="22" t="s">
+      <c r="D118" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E118" s="5" t="s">
@@ -5915,7 +5932,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K118" s="14" t="s">
+      <c r="K118" t="s">
         <v>371</v>
       </c>
       <c r="L118" s="5" t="s">
@@ -5926,13 +5943,13 @@
       <c r="A119" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B119" s="14" t="s">
+      <c r="B119" t="s">
         <v>56</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D119" s="22" t="s">
+      <c r="D119" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E119" s="5" t="s">
@@ -5945,7 +5962,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K119" s="14" t="s">
+      <c r="K119" t="s">
         <v>371</v>
       </c>
       <c r="L119" s="5" t="s">
@@ -5956,13 +5973,13 @@
       <c r="A120" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B120" s="14" t="s">
+      <c r="B120" t="s">
         <v>56</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D120" s="22" t="s">
+      <c r="D120" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E120" s="5" t="s">
@@ -5975,7 +5992,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K120" s="14" t="s">
+      <c r="K120" t="s">
         <v>371</v>
       </c>
       <c r="L120" s="5" t="s">
@@ -5986,13 +6003,13 @@
       <c r="A121" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B121" s="14" t="s">
+      <c r="B121" t="s">
         <v>56</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D121" s="22" t="s">
+      <c r="D121" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E121" s="5" t="s">
@@ -6005,7 +6022,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K121" s="14" t="s">
+      <c r="K121" t="s">
         <v>371</v>
       </c>
       <c r="L121" s="5" t="s">
@@ -6016,13 +6033,13 @@
       <c r="A122" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="B122" t="s">
         <v>56</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D122" s="22" t="s">
+      <c r="D122" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E122" s="5" t="s">
@@ -6035,7 +6052,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K122" s="14" t="s">
+      <c r="K122" t="s">
         <v>371</v>
       </c>
       <c r="L122" s="5" t="s">
@@ -6046,13 +6063,13 @@
       <c r="A123" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="B123" t="s">
         <v>56</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D123" s="22" t="s">
+      <c r="D123" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E123" s="5" t="s">
@@ -6065,7 +6082,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K123" s="14" t="s">
+      <c r="K123" t="s">
         <v>371</v>
       </c>
       <c r="L123" s="5" t="s">
@@ -6076,13 +6093,13 @@
       <c r="A124" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B124" s="14" t="s">
+      <c r="B124" t="s">
         <v>56</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="D124" s="22" t="s">
+      <c r="D124" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E124" s="5" t="s">
@@ -6095,7 +6112,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K124" s="14" t="s">
+      <c r="K124" t="s">
         <v>371</v>
       </c>
       <c r="L124" s="5" t="s">
@@ -6106,13 +6123,13 @@
       <c r="A125" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B125" s="14" t="s">
+      <c r="B125" t="s">
         <v>56</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D125" s="22" t="s">
+      <c r="D125" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E125" s="5" t="s">
@@ -6125,7 +6142,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K125" s="14" t="s">
+      <c r="K125" t="s">
         <v>371</v>
       </c>
       <c r="L125" s="5" t="s">
@@ -6136,13 +6153,13 @@
       <c r="A126" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B126" s="14" t="s">
+      <c r="B126" t="s">
         <v>56</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="D126" s="22" t="s">
+      <c r="D126" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E126" s="5" t="s">
@@ -6155,7 +6172,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K126" s="14" t="s">
+      <c r="K126" t="s">
         <v>371</v>
       </c>
       <c r="L126" s="5" t="s">
@@ -6166,13 +6183,13 @@
       <c r="A127" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B127" s="14" t="s">
+      <c r="B127" t="s">
         <v>56</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D127" s="22" t="s">
+      <c r="D127" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E127" s="5" t="s">
@@ -6185,7 +6202,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K127" s="14" t="s">
+      <c r="K127" t="s">
         <v>371</v>
       </c>
       <c r="L127" s="5" t="s">
@@ -6196,13 +6213,13 @@
       <c r="A128" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B128" s="14" t="s">
+      <c r="B128" t="s">
         <v>56</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D128" s="22" t="s">
+      <c r="D128" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E128" s="5" t="s">
@@ -6215,7 +6232,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K128" s="14" t="s">
+      <c r="K128" t="s">
         <v>371</v>
       </c>
       <c r="L128" s="5" t="s">
@@ -6226,13 +6243,13 @@
       <c r="A129" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B129" t="s">
         <v>56</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D129" s="22" t="s">
+      <c r="D129" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E129" s="5" t="s">
@@ -6245,7 +6262,7 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K129" s="14" t="s">
+      <c r="K129" t="s">
         <v>371</v>
       </c>
       <c r="L129" s="5" t="s">
@@ -6253,7 +6270,7 @@
       </c>
     </row>
     <row r="130" spans="1:12">
-      <c r="A130" s="15" t="s">
+      <c r="A130" s="5" t="s">
         <v>496</v>
       </c>
       <c r="B130" s="5" t="s">
@@ -6262,7 +6279,7 @@
       <c r="C130" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D130" s="22" t="s">
+      <c r="D130" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E130" s="5" t="s">
@@ -6285,7 +6302,7 @@
       </c>
     </row>
     <row r="131" spans="1:12" ht="30">
-      <c r="A131" s="15" t="s">
+      <c r="A131" s="5" t="s">
         <v>497</v>
       </c>
       <c r="B131" s="5" t="s">
@@ -6294,7 +6311,7 @@
       <c r="C131" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="D131" s="22" t="s">
+      <c r="D131" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E131" s="5" t="s">
@@ -6317,7 +6334,7 @@
       </c>
     </row>
     <row r="132" spans="1:12">
-      <c r="A132" s="15" t="s">
+      <c r="A132" s="5" t="s">
         <v>498</v>
       </c>
       <c r="B132" s="5" t="s">
@@ -6326,7 +6343,7 @@
       <c r="C132" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="D132" s="22" t="s">
+      <c r="D132" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E132" s="5" t="s">
@@ -6349,7 +6366,7 @@
       </c>
     </row>
     <row r="133" spans="1:12" ht="30">
-      <c r="A133" s="15" t="s">
+      <c r="A133" s="5" t="s">
         <v>499</v>
       </c>
       <c r="B133" s="5" t="s">
@@ -6358,7 +6375,7 @@
       <c r="C133" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="D133" s="22" t="s">
+      <c r="D133" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E133" s="5" t="s">
@@ -6390,7 +6407,7 @@
       <c r="C134" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="D134" s="22" t="s">
+      <c r="D134" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E134" s="5" t="s">
@@ -6419,7 +6436,7 @@
       <c r="C135" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D135" s="22" t="s">
+      <c r="D135" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E135" s="5" t="s">
@@ -6448,7 +6465,7 @@
       <c r="C136" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="D136" s="22" t="s">
+      <c r="D136" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E136" s="5" t="s">
@@ -6477,7 +6494,7 @@
       <c r="C137" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="D137" s="22" t="s">
+      <c r="D137" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E137" s="5" t="s">
@@ -6506,7 +6523,7 @@
       <c r="C138" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="D138" s="22" t="s">
+      <c r="D138" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E138" s="5" t="s">
@@ -6535,7 +6552,7 @@
       <c r="C139" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="D139" s="22" t="s">
+      <c r="D139" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E139" s="5" t="s">
@@ -6564,7 +6581,7 @@
       <c r="C140" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="D140" s="22" t="s">
+      <c r="D140" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E140" s="5" t="s">
@@ -6593,7 +6610,7 @@
       <c r="C141" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="D141" s="22" t="s">
+      <c r="D141" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E141" s="5" t="s">
@@ -6622,7 +6639,7 @@
       <c r="C142" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="D142" s="22" t="s">
+      <c r="D142" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E142" s="5" t="s">
@@ -6651,7 +6668,7 @@
       <c r="C143" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D143" s="22" t="s">
+      <c r="D143" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E143" s="5" t="s">
@@ -6680,7 +6697,7 @@
       <c r="C144" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D144" s="22" t="s">
+      <c r="D144" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E144" s="5" t="s">
@@ -6709,7 +6726,7 @@
       <c r="C145" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D145" s="22" t="s">
+      <c r="D145" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E145" s="5" t="s">
@@ -6738,7 +6755,7 @@
       <c r="C146" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="D146" s="22" t="s">
+      <c r="D146" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E146" s="5" t="s">
@@ -6767,7 +6784,7 @@
       <c r="C147" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="D147" s="22" t="s">
+      <c r="D147" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E147" s="5" t="s">
@@ -6796,7 +6813,7 @@
       <c r="C148" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="D148" s="22" t="s">
+      <c r="D148" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E148" s="5" t="s">
@@ -6825,7 +6842,7 @@
       <c r="C149" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="D149" s="22" t="s">
+      <c r="D149" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E149" s="5" t="s">
@@ -6854,7 +6871,7 @@
       <c r="C150" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="D150" s="22" t="s">
+      <c r="D150" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E150" s="5" t="s">
@@ -6883,7 +6900,7 @@
       <c r="C151" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="D151" s="22" t="s">
+      <c r="D151" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E151" s="5" t="s">
@@ -6912,7 +6929,7 @@
       <c r="C152" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="D152" s="22" t="s">
+      <c r="D152" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E152" s="5" t="s">
@@ -6941,7 +6958,7 @@
       <c r="C153" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="D153" s="22" t="s">
+      <c r="D153" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E153" s="5" t="s">
@@ -6970,7 +6987,7 @@
       <c r="C154" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="D154" s="22" t="s">
+      <c r="D154" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E154" s="5" t="s">
@@ -6999,7 +7016,7 @@
       <c r="C155" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="D155" s="22" t="s">
+      <c r="D155" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E155" s="5" t="s">
@@ -7028,7 +7045,7 @@
       <c r="C156" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="D156" s="22" t="s">
+      <c r="D156" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E156" s="5" t="s">
@@ -7057,7 +7074,7 @@
       <c r="C157" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="D157" s="22" t="s">
+      <c r="D157" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E157" s="5" t="s">
@@ -7086,7 +7103,7 @@
       <c r="C158" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="D158" s="22" t="s">
+      <c r="D158" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E158" s="5" t="s">
@@ -7115,7 +7132,7 @@
       <c r="C159" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="D159" s="22" t="s">
+      <c r="D159" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E159" s="5" t="s">
@@ -7144,7 +7161,7 @@
       <c r="C160" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="D160" s="22" t="s">
+      <c r="D160" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E160" s="5" t="s">
@@ -7173,7 +7190,7 @@
       <c r="C161" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D161" s="22" t="s">
+      <c r="D161" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E161" s="5" t="s">
@@ -7202,7 +7219,7 @@
       <c r="C162" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="D162" s="22" t="s">
+      <c r="D162" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E162" s="5" t="s">
@@ -7231,7 +7248,7 @@
       <c r="C163" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="D163" s="22" t="s">
+      <c r="D163" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E163" s="5" t="s">
@@ -7260,7 +7277,7 @@
       <c r="C164" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="D164" s="22" t="s">
+      <c r="D164" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E164" s="5" t="s">
@@ -7289,7 +7306,7 @@
       <c r="C165" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="D165" s="22" t="s">
+      <c r="D165" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E165" s="5" t="s">
@@ -7318,7 +7335,7 @@
       <c r="C166" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="D166" s="22" t="s">
+      <c r="D166" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E166" s="5" t="s">
@@ -7347,7 +7364,7 @@
       <c r="C167" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="D167" s="22" t="s">
+      <c r="D167" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E167" s="5" t="s">
@@ -7376,7 +7393,7 @@
       <c r="C168" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="D168" s="22" t="s">
+      <c r="D168" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E168" s="5" t="s">
@@ -7405,7 +7422,7 @@
       <c r="C169" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="D169" s="22" t="s">
+      <c r="D169" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E169" s="5" t="s">
@@ -7434,7 +7451,7 @@
       <c r="C170" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="D170" s="22" t="s">
+      <c r="D170" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E170" s="5" t="s">
@@ -7463,7 +7480,7 @@
       <c r="C171" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="D171" s="22" t="s">
+      <c r="D171" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E171" s="5" t="s">
@@ -7492,7 +7509,7 @@
       <c r="C172" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="D172" s="22" t="s">
+      <c r="D172" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E172" s="5" t="s">
@@ -7521,7 +7538,7 @@
       <c r="C173" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="D173" s="22" t="s">
+      <c r="D173" s="19" t="s">
         <v>299</v>
       </c>
       <c r="E173" s="5" t="s">
@@ -7550,7 +7567,7 @@
       <c r="C174" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D174" s="22" t="s">
+      <c r="D174" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E174" s="5" t="s">
@@ -7579,7 +7596,7 @@
       <c r="C175" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="D175" s="22" t="s">
+      <c r="D175" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E175" s="5" t="s">
@@ -7608,7 +7625,7 @@
       <c r="C176" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="D176" s="22" t="s">
+      <c r="D176" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E176" s="5" t="s">
@@ -7637,7 +7654,7 @@
       <c r="C177" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="D177" s="22" t="s">
+      <c r="D177" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E177" s="5" t="s">
@@ -7666,7 +7683,7 @@
       <c r="C178" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="D178" s="22" t="s">
+      <c r="D178" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E178" s="5" t="s">
@@ -7695,7 +7712,7 @@
       <c r="C179" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="D179" s="22" t="s">
+      <c r="D179" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E179" s="5" t="s">
@@ -7724,7 +7741,7 @@
       <c r="C180" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="D180" s="22" t="s">
+      <c r="D180" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E180" s="5" t="s">
@@ -7753,7 +7770,7 @@
       <c r="C181" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="D181" s="22" t="s">
+      <c r="D181" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E181" s="5" t="s">
@@ -7782,7 +7799,7 @@
       <c r="C182" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="D182" s="22" t="s">
+      <c r="D182" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E182" s="5" t="s">
@@ -7797,7 +7814,7 @@
       <c r="K182" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="L182" s="24" t="s">
+      <c r="L182" s="21" t="s">
         <v>470</v>
       </c>
     </row>
@@ -7811,7 +7828,7 @@
       <c r="C183" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="D183" s="22" t="s">
+      <c r="D183" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E183" s="5" t="s">
@@ -7826,7 +7843,7 @@
       <c r="K183" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="L183" s="23" t="s">
+      <c r="L183" s="20" t="s">
         <v>468</v>
       </c>
     </row>
@@ -7840,7 +7857,7 @@
       <c r="C184" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="D184" s="22" t="s">
+      <c r="D184" s="19" t="s">
         <v>448</v>
       </c>
       <c r="E184" s="5" t="s">
@@ -7855,7 +7872,7 @@
       <c r="K184" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="L184" s="23" t="s">
+      <c r="L184" s="20" t="s">
         <v>469</v>
       </c>
     </row>
@@ -7869,7 +7886,7 @@
       <c r="C185" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="D185" s="21" t="s">
+      <c r="D185" s="18" t="s">
         <v>476</v>
       </c>
       <c r="E185" s="5" t="s">
@@ -7898,7 +7915,7 @@
       <c r="C186" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="D186" s="21" t="s">
+      <c r="D186" s="18" t="s">
         <v>476</v>
       </c>
       <c r="E186" s="5" t="s">
@@ -7927,7 +7944,7 @@
       <c r="C187" s="5" t="s">
         <v>514</v>
       </c>
-      <c r="D187" s="21" t="s">
+      <c r="D187" s="18" t="s">
         <v>476</v>
       </c>
       <c r="E187" s="5" t="s">
@@ -7948,6 +7965,134 @@
       </c>
       <c r="L187" s="7" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" ht="30">
+      <c r="A188" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="D188" s="18" t="s">
+        <v>521</v>
+      </c>
+      <c r="E188" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="H188" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="I188" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J188" s="5">
+        <v>3</v>
+      </c>
+      <c r="K188" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L188" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" ht="30">
+      <c r="A189" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="D189" s="18" t="s">
+        <v>521</v>
+      </c>
+      <c r="E189" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="H189" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="I189" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J189" s="5">
+        <v>3</v>
+      </c>
+      <c r="K189" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L189" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" ht="30">
+      <c r="A190" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="D190" s="18" t="s">
+        <v>521</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="H190" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="I190" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J190" s="5">
+        <v>3</v>
+      </c>
+      <c r="K190" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L190" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
+      <c r="A191" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C191" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="D191" s="18" t="s">
+        <v>521</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="H191" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="I191" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J191" s="5">
+        <v>3</v>
+      </c>
+      <c r="K191" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L191" s="5" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>